<commit_message>
3ra Entrega SIBEN 2022
</commit_message>
<xml_diff>
--- a/003_BasesNiveles/V003_17Mayo2022/001_EXCEL/002_BE_Niveles IPT.xlsx
+++ b/003_BasesNiveles/V003_17Mayo2022/001_EXCEL/002_BE_Niveles IPT.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EB30"/>
+  <dimension ref="A1:EC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1018,6 +1018,11 @@
           <t>Inf_tardias_10_ARM</t>
         </is>
       </c>
+      <c r="EC1" s="1" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1676,6 +1681,11 @@
         </is>
       </c>
       <c r="EB2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="EC2" t="inlineStr">
         <is>
           <t>NO</t>
         </is>

</xml_diff>